<commit_message>
Add sheets of growth rate in MEA and PEA demands
</commit_message>
<xml_diff>
--- a/process_data/excel_control.xlsx
+++ b/process_data/excel_control.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rstudio\load_forecast_EGAT_strategies\process_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DE301D-9CA5-48AE-8A51-95A4B473D250}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D7B63C-464B-4CEB-AE37-68E8C5A6964A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{20F41227-94A0-4EEA-A92D-3A5CF9DBE630}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2" xr2:uid="{20F41227-94A0-4EEA-A92D-3A5CF9DBE630}"/>
   </bookViews>
   <sheets>
     <sheet name="grw_3u" sheetId="1" r:id="rId1"/>
+    <sheet name="grw_mea_dmd" sheetId="2" r:id="rId2"/>
+    <sheet name="grw_pea_dmd" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
   <si>
     <t>year</t>
   </si>
@@ -394,8 +396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85327E8-F140-40CE-89AE-80876F2A21BF}">
   <dimension ref="A1:B83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B6:B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -959,4 +961,1146 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7F06DE-0687-42DF-9DC2-BCCD5FE1CFB4}">
+  <dimension ref="A1:B83"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2019</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2020</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2021</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2022</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2023</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" ref="B6:B20" si="0">1-0.0113</f>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2024</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2025</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2026</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2027</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2028</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2029</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2030</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2031</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2032</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2033</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2034</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2035</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2036</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2037</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2038</v>
+      </c>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2039</v>
+      </c>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2040</v>
+      </c>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2041</v>
+      </c>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2042</v>
+      </c>
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2043</v>
+      </c>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2044</v>
+      </c>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2045</v>
+      </c>
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2046</v>
+      </c>
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2047</v>
+      </c>
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2048</v>
+      </c>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2049</v>
+      </c>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2050</v>
+      </c>
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2051</v>
+      </c>
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2052</v>
+      </c>
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>2053</v>
+      </c>
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2054</v>
+      </c>
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2055</v>
+      </c>
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2056</v>
+      </c>
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2057</v>
+      </c>
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>2058</v>
+      </c>
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>2059</v>
+      </c>
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2060</v>
+      </c>
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2061</v>
+      </c>
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2062</v>
+      </c>
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2063</v>
+      </c>
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2064</v>
+      </c>
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2065</v>
+      </c>
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>2066</v>
+      </c>
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2067</v>
+      </c>
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>2068</v>
+      </c>
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>2069</v>
+      </c>
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>2070</v>
+      </c>
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>2071</v>
+      </c>
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>2072</v>
+      </c>
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>2073</v>
+      </c>
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>2074</v>
+      </c>
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>2075</v>
+      </c>
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>2076</v>
+      </c>
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>2077</v>
+      </c>
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>2078</v>
+      </c>
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>2079</v>
+      </c>
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>2080</v>
+      </c>
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>2081</v>
+      </c>
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>2082</v>
+      </c>
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>2083</v>
+      </c>
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>2084</v>
+      </c>
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>2085</v>
+      </c>
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>2086</v>
+      </c>
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>2087</v>
+      </c>
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>2088</v>
+      </c>
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>2089</v>
+      </c>
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>2090</v>
+      </c>
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>2091</v>
+      </c>
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>2092</v>
+      </c>
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>2093</v>
+      </c>
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>2094</v>
+      </c>
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>2095</v>
+      </c>
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>2096</v>
+      </c>
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>2097</v>
+      </c>
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>2098</v>
+      </c>
+      <c r="B81" s="1"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>2099</v>
+      </c>
+      <c r="B82" s="1"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>2100</v>
+      </c>
+      <c r="B83" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D9E9F3-C524-4792-89E7-671C9C67DF88}">
+  <dimension ref="A1:B83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2019</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2020</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2021</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2022</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2023</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" ref="B6:B20" si="0">1-0.0113</f>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2024</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2025</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2026</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2027</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2028</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2029</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2030</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2031</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2032</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2033</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2034</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2035</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2036</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2037</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2038</v>
+      </c>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2039</v>
+      </c>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2040</v>
+      </c>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2041</v>
+      </c>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2042</v>
+      </c>
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2043</v>
+      </c>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2044</v>
+      </c>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2045</v>
+      </c>
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2046</v>
+      </c>
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2047</v>
+      </c>
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2048</v>
+      </c>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2049</v>
+      </c>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2050</v>
+      </c>
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2051</v>
+      </c>
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2052</v>
+      </c>
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>2053</v>
+      </c>
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2054</v>
+      </c>
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2055</v>
+      </c>
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2056</v>
+      </c>
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2057</v>
+      </c>
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>2058</v>
+      </c>
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>2059</v>
+      </c>
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2060</v>
+      </c>
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2061</v>
+      </c>
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2062</v>
+      </c>
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2063</v>
+      </c>
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2064</v>
+      </c>
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2065</v>
+      </c>
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>2066</v>
+      </c>
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2067</v>
+      </c>
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>2068</v>
+      </c>
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>2069</v>
+      </c>
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>2070</v>
+      </c>
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>2071</v>
+      </c>
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>2072</v>
+      </c>
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>2073</v>
+      </c>
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>2074</v>
+      </c>
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>2075</v>
+      </c>
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>2076</v>
+      </c>
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>2077</v>
+      </c>
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>2078</v>
+      </c>
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>2079</v>
+      </c>
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>2080</v>
+      </c>
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>2081</v>
+      </c>
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>2082</v>
+      </c>
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>2083</v>
+      </c>
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>2084</v>
+      </c>
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>2085</v>
+      </c>
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>2086</v>
+      </c>
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>2087</v>
+      </c>
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>2088</v>
+      </c>
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>2089</v>
+      </c>
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>2090</v>
+      </c>
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>2091</v>
+      </c>
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>2092</v>
+      </c>
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>2093</v>
+      </c>
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>2094</v>
+      </c>
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>2095</v>
+      </c>
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>2096</v>
+      </c>
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>2097</v>
+      </c>
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>2098</v>
+      </c>
+      <c r="B81" s="1"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>2099</v>
+      </c>
+      <c r="B82" s="1"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>2100</v>
+      </c>
+      <c r="B83" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Edit the growth rate
</commit_message>
<xml_diff>
--- a/process_data/excel_control.xlsx
+++ b/process_data/excel_control.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rstudio\load_forecast_EGAT_strategies\process_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D7B63C-464B-4CEB-AE37-68E8C5A6964A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2E83AA-F9B2-4C31-BFA8-2C6A2EF92739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2" xr2:uid="{20F41227-94A0-4EEA-A92D-3A5CF9DBE630}"/>
+    <workbookView xWindow="3276" yWindow="3276" windowWidth="11040" windowHeight="8964" xr2:uid="{20F41227-94A0-4EEA-A92D-3A5CF9DBE630}"/>
   </bookViews>
   <sheets>
     <sheet name="grw_3u" sheetId="1" r:id="rId1"/>
@@ -43,14 +43,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -396,16 +396,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85327E8-F140-40CE-89AE-80876F2A21BF}">
   <dimension ref="A1:B83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,546 +413,531 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2019</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2020</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2021</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2022</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2023</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" ref="B6:B8" si="0">1-0.0113</f>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2024</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2025</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2026</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" ref="B9:B20" si="1">1-0.0113</f>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2027</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="1"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2028</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="1"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2029</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="1"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2030</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="1"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2031</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="1"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2032</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="1"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2033</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" si="1"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2034</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="1"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2035</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="1"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2036</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="1"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2037</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="1"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2038</v>
       </c>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2039</v>
       </c>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2040</v>
       </c>
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2041</v>
       </c>
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2042</v>
       </c>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2043</v>
       </c>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2044</v>
       </c>
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2045</v>
       </c>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2046</v>
       </c>
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2047</v>
       </c>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2048</v>
       </c>
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2049</v>
       </c>
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2050</v>
       </c>
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2051</v>
       </c>
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2052</v>
       </c>
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2053</v>
       </c>
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2054</v>
       </c>
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2055</v>
       </c>
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2056</v>
       </c>
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2057</v>
       </c>
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2058</v>
       </c>
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2059</v>
       </c>
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2060</v>
       </c>
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2061</v>
       </c>
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2062</v>
       </c>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2063</v>
       </c>
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2064</v>
       </c>
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2065</v>
       </c>
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2066</v>
       </c>
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2067</v>
       </c>
       <c r="B50" s="1"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2068</v>
       </c>
       <c r="B51" s="1"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2069</v>
       </c>
       <c r="B52" s="1"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2070</v>
       </c>
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2071</v>
       </c>
       <c r="B54" s="1"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2072</v>
       </c>
       <c r="B55" s="1"/>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2073</v>
       </c>
       <c r="B56" s="1"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2074</v>
       </c>
       <c r="B57" s="1"/>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2075</v>
       </c>
       <c r="B58" s="1"/>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2076</v>
       </c>
       <c r="B59" s="1"/>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2077</v>
       </c>
       <c r="B60" s="1"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2078</v>
       </c>
       <c r="B61" s="1"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2079</v>
       </c>
       <c r="B62" s="1"/>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2080</v>
       </c>
       <c r="B63" s="1"/>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2081</v>
       </c>
       <c r="B64" s="1"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2082</v>
       </c>
       <c r="B65" s="1"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2083</v>
       </c>
       <c r="B66" s="1"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2084</v>
       </c>
       <c r="B67" s="1"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2085</v>
       </c>
       <c r="B68" s="1"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2086</v>
       </c>
       <c r="B69" s="1"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2087</v>
       </c>
       <c r="B70" s="1"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2088</v>
       </c>
       <c r="B71" s="1"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2089</v>
       </c>
       <c r="B72" s="1"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2090</v>
       </c>
       <c r="B73" s="1"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>2091</v>
       </c>
       <c r="B74" s="1"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>2092</v>
       </c>
       <c r="B75" s="1"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2093</v>
       </c>
       <c r="B76" s="1"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2094</v>
       </c>
       <c r="B77" s="1"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>2095</v>
       </c>
       <c r="B78" s="1"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2096</v>
       </c>
       <c r="B79" s="1"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>2097</v>
       </c>
       <c r="B80" s="1"/>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>2098</v>
       </c>
       <c r="B81" s="1"/>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>2099</v>
       </c>
       <c r="B82" s="1"/>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>2100</v>
       </c>
@@ -967,16 +952,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7F06DE-0687-42DF-9DC2-BCCD5FE1CFB4}">
   <dimension ref="A1:B83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -984,546 +969,531 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2019</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2020</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2021</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2022</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2023</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" ref="B6:B20" si="0">1-0.0113</f>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2024</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2025</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2026</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2027</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2028</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2029</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2030</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2031</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2032</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2033</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2034</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2035</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2036</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2037</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2038</v>
       </c>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2039</v>
       </c>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2040</v>
       </c>
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2041</v>
       </c>
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2042</v>
       </c>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2043</v>
       </c>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2044</v>
       </c>
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2045</v>
       </c>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2046</v>
       </c>
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2047</v>
       </c>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2048</v>
       </c>
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2049</v>
       </c>
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2050</v>
       </c>
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2051</v>
       </c>
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2052</v>
       </c>
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2053</v>
       </c>
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2054</v>
       </c>
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2055</v>
       </c>
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2056</v>
       </c>
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2057</v>
       </c>
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2058</v>
       </c>
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2059</v>
       </c>
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2060</v>
       </c>
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2061</v>
       </c>
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2062</v>
       </c>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2063</v>
       </c>
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2064</v>
       </c>
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2065</v>
       </c>
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2066</v>
       </c>
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2067</v>
       </c>
       <c r="B50" s="1"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2068</v>
       </c>
       <c r="B51" s="1"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2069</v>
       </c>
       <c r="B52" s="1"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2070</v>
       </c>
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2071</v>
       </c>
       <c r="B54" s="1"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2072</v>
       </c>
       <c r="B55" s="1"/>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2073</v>
       </c>
       <c r="B56" s="1"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2074</v>
       </c>
       <c r="B57" s="1"/>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2075</v>
       </c>
       <c r="B58" s="1"/>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2076</v>
       </c>
       <c r="B59" s="1"/>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2077</v>
       </c>
       <c r="B60" s="1"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2078</v>
       </c>
       <c r="B61" s="1"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2079</v>
       </c>
       <c r="B62" s="1"/>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2080</v>
       </c>
       <c r="B63" s="1"/>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2081</v>
       </c>
       <c r="B64" s="1"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2082</v>
       </c>
       <c r="B65" s="1"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2083</v>
       </c>
       <c r="B66" s="1"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2084</v>
       </c>
       <c r="B67" s="1"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2085</v>
       </c>
       <c r="B68" s="1"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2086</v>
       </c>
       <c r="B69" s="1"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2087</v>
       </c>
       <c r="B70" s="1"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2088</v>
       </c>
       <c r="B71" s="1"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2089</v>
       </c>
       <c r="B72" s="1"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2090</v>
       </c>
       <c r="B73" s="1"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>2091</v>
       </c>
       <c r="B74" s="1"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>2092</v>
       </c>
       <c r="B75" s="1"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2093</v>
       </c>
       <c r="B76" s="1"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2094</v>
       </c>
       <c r="B77" s="1"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>2095</v>
       </c>
       <c r="B78" s="1"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2096</v>
       </c>
       <c r="B79" s="1"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>2097</v>
       </c>
       <c r="B80" s="1"/>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>2098</v>
       </c>
       <c r="B81" s="1"/>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>2099</v>
       </c>
       <c r="B82" s="1"/>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>2100</v>
       </c>
@@ -1538,16 +1508,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D9E9F3-C524-4792-89E7-671C9C67DF88}">
   <dimension ref="A1:B83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1555,546 +1525,531 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2019</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2020</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2021</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2022</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2023</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" ref="B6:B20" si="0">1-0.0113</f>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2024</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2025</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2026</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2027</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2028</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2029</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2030</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2031</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2032</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2033</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2034</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2035</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2036</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2037</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2038</v>
       </c>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2039</v>
       </c>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2040</v>
       </c>
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2041</v>
       </c>
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2042</v>
       </c>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2043</v>
       </c>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2044</v>
       </c>
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2045</v>
       </c>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2046</v>
       </c>
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2047</v>
       </c>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2048</v>
       </c>
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2049</v>
       </c>
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2050</v>
       </c>
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2051</v>
       </c>
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2052</v>
       </c>
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2053</v>
       </c>
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2054</v>
       </c>
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2055</v>
       </c>
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2056</v>
       </c>
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2057</v>
       </c>
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2058</v>
       </c>
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2059</v>
       </c>
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2060</v>
       </c>
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2061</v>
       </c>
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2062</v>
       </c>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2063</v>
       </c>
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2064</v>
       </c>
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2065</v>
       </c>
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2066</v>
       </c>
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2067</v>
       </c>
       <c r="B50" s="1"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2068</v>
       </c>
       <c r="B51" s="1"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2069</v>
       </c>
       <c r="B52" s="1"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2070</v>
       </c>
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2071</v>
       </c>
       <c r="B54" s="1"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2072</v>
       </c>
       <c r="B55" s="1"/>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2073</v>
       </c>
       <c r="B56" s="1"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2074</v>
       </c>
       <c r="B57" s="1"/>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2075</v>
       </c>
       <c r="B58" s="1"/>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2076</v>
       </c>
       <c r="B59" s="1"/>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2077</v>
       </c>
       <c r="B60" s="1"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2078</v>
       </c>
       <c r="B61" s="1"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2079</v>
       </c>
       <c r="B62" s="1"/>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2080</v>
       </c>
       <c r="B63" s="1"/>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2081</v>
       </c>
       <c r="B64" s="1"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2082</v>
       </c>
       <c r="B65" s="1"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2083</v>
       </c>
       <c r="B66" s="1"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2084</v>
       </c>
       <c r="B67" s="1"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2085</v>
       </c>
       <c r="B68" s="1"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2086</v>
       </c>
       <c r="B69" s="1"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2087</v>
       </c>
       <c r="B70" s="1"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2088</v>
       </c>
       <c r="B71" s="1"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2089</v>
       </c>
       <c r="B72" s="1"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2090</v>
       </c>
       <c r="B73" s="1"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>2091</v>
       </c>
       <c r="B74" s="1"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>2092</v>
       </c>
       <c r="B75" s="1"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2093</v>
       </c>
       <c r="B76" s="1"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2094</v>
       </c>
       <c r="B77" s="1"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>2095</v>
       </c>
       <c r="B78" s="1"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2096</v>
       </c>
       <c r="B79" s="1"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>2097</v>
       </c>
       <c r="B80" s="1"/>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>2098</v>
       </c>
       <c r="B81" s="1"/>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>2099</v>
       </c>
       <c r="B82" s="1"/>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>2100</v>
       </c>

</xml_diff>